<commit_message>
update for Excel method
</commit_message>
<xml_diff>
--- a/TPMS-param.xlsx
+++ b/TPMS-param.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2024\BoboSlicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A153E-65FE-447F-87A0-52AB41330C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64090908-3DBD-48C9-9469-134B1EE02701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="3495" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7035" yWindow="2685" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANTest" sheetId="1" r:id="rId1"/>
+    <sheet name="ANTest_wi_padding" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Type</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>FKSolid</t>
+  </si>
+  <si>
+    <t>xPadding</t>
+  </si>
+  <si>
+    <t>yPadding</t>
+  </si>
+  <si>
+    <t>FKSSolid</t>
   </si>
 </sst>
 </file>
@@ -372,22 +382,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -406,8 +417,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -426,8 +443,14 @@
       <c r="F2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -435,7 +458,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0.61629999999999996</v>
@@ -447,8 +470,14 @@
         <f>25+35</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -468,8 +497,14 @@
         <f>25+70</f>
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -477,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0.40379999999999999</v>
@@ -489,8 +524,14 @@
         <f>25+35+70</f>
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -509,8 +550,14 @@
       <c r="F6">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -530,8 +577,14 @@
         <f>25+35</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -551,8 +604,14 @@
         <f>25+70</f>
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -571,6 +630,276 @@
       <c r="F9">
         <f>25+35+70</f>
         <v>130</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817271C1-A6B4-459A-98A5-941B6348E759}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0.61629999999999996</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.61629999999999996</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <f>25+35</f>
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>0.40379999999999999</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <f>25+70</f>
+        <v>95</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0.40379999999999999</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <f>25+35+70</f>
+        <v>130</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.46410000000000001</v>
+      </c>
+      <c r="E6">
+        <v>185</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0.46410000000000001</v>
+      </c>
+      <c r="E7">
+        <v>185</v>
+      </c>
+      <c r="F7">
+        <f>25+35</f>
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="E8">
+        <v>185</v>
+      </c>
+      <c r="F8">
+        <f>25+70</f>
+        <v>95</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="E9">
+        <v>185</v>
+      </c>
+      <c r="F9">
+        <f>25+35+70</f>
+        <v>130</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
For calculating the volume fraction.
</commit_message>
<xml_diff>
--- a/TPMS-param.xlsx
+++ b/TPMS-param.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2024\BoboSlicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13E9395-2503-489F-AE79-2D322BC84D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33100B4-DEE7-40B9-85B3-8F3F5871EB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7035" yWindow="2685" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ANTest" sheetId="1" r:id="rId1"/>
-    <sheet name="ANTest_wi_padding" sheetId="2" r:id="rId2"/>
+    <sheet name="ANTest_wi_padding" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -56,6 +55,15 @@
   </si>
   <si>
     <t>FKSSolid</t>
+  </si>
+  <si>
+    <t>xAxisLength</t>
+  </si>
+  <si>
+    <t>yAxisLength</t>
+  </si>
+  <si>
+    <t>zAxisLength</t>
   </si>
   <si>
     <t>xSeal</t>
@@ -378,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817271C1-A6B4-459A-98A5-941B6348E759}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,9 +401,10 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -415,13 +424,22 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -441,13 +459,22 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>120</v>
+      </c>
+      <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,13 +495,22 @@
         <v>60</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -495,13 +531,22 @@
         <v>95</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>120</v>
+      </c>
+      <c r="J4">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -522,13 +567,22 @@
         <v>130</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>120</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -548,13 +602,22 @@
         <v>25</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>120</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -575,13 +638,22 @@
         <v>60</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>120</v>
+      </c>
+      <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -602,13 +674,22 @@
         <v>95</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>120</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -629,274 +710,19 @@
         <v>130</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817271C1-A6B4-459A-98A5-941B6348E759}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0.61629999999999996</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0.61629999999999996</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <f>25+35</f>
-        <v>60</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>0.40379999999999999</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <f>25+70</f>
-        <v>95</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>0.40379999999999999</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <f>25+35+70</f>
-        <v>130</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>0.46410000000000001</v>
-      </c>
-      <c r="E6">
-        <v>185</v>
-      </c>
-      <c r="F6">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0.46410000000000001</v>
-      </c>
-      <c r="E7">
-        <v>185</v>
-      </c>
-      <c r="F7">
-        <f>25+35</f>
-        <v>60</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>0.30459999999999998</v>
-      </c>
-      <c r="E8">
-        <v>185</v>
-      </c>
-      <c r="F8">
-        <f>25+70</f>
-        <v>95</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>0.30459999999999998</v>
-      </c>
-      <c r="E9">
-        <v>185</v>
-      </c>
-      <c r="F9">
-        <f>25+35+70</f>
-        <v>130</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
+      <c r="I9">
+        <v>120</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>